<commit_message>
Aufwands- und Terminplan aktualisiert
</commit_message>
<xml_diff>
--- a/Doku/Managementplaene_und_listen.xlsx
+++ b/Doku/Managementplaene_und_listen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="323">
   <si>
     <t>Risikoliste</t>
   </si>
@@ -1248,6 +1248,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1276,9 +1279,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2373,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3255,10 +3255,12 @@
         <v>290</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="1">
+        <v>3</v>
+      </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,10 +3272,12 @@
         <v>291</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="1">
+        <v>3</v>
+      </c>
       <c r="F52" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,10 +3289,12 @@
         <v>293</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="E53" s="1">
+        <v>3</v>
+      </c>
       <c r="F53" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3431,10 +3437,12 @@
       <c r="D62" s="1">
         <v>12</v>
       </c>
-      <c r="E62" s="1"/>
+      <c r="E62" s="1">
+        <v>12</v>
+      </c>
       <c r="F62" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3448,10 +3456,12 @@
       <c r="D63" s="1">
         <v>12</v>
       </c>
-      <c r="E63" s="1"/>
+      <c r="E63" s="1">
+        <v>12</v>
+      </c>
       <c r="F63" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3465,10 +3475,12 @@
       <c r="D64" s="1">
         <v>12</v>
       </c>
-      <c r="E64" s="1"/>
+      <c r="E64" s="1">
+        <v>12</v>
+      </c>
       <c r="F64" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3482,10 +3494,12 @@
       <c r="D65" s="1">
         <v>12</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1">
+        <v>12</v>
+      </c>
       <c r="F65" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3499,10 +3513,12 @@
       <c r="D66" s="1">
         <v>12</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1">
+        <v>12</v>
+      </c>
       <c r="F66" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3516,10 +3532,12 @@
       <c r="D67" s="1">
         <v>12</v>
       </c>
-      <c r="E67" s="1"/>
+      <c r="E67" s="1">
+        <v>2</v>
+      </c>
       <c r="F67" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -3568,11 +3586,11 @@
         <v>22</v>
       </c>
       <c r="E70" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -4065,7 +4083,7 @@
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C114" s="41" t="s">
+      <c r="C114" s="31" t="s">
         <v>297</v>
       </c>
       <c r="D114" s="2">
@@ -4074,11 +4092,11 @@
       </c>
       <c r="E114" s="2">
         <f>SUM(E3:E113)</f>
-        <v>233</v>
+        <v>312</v>
       </c>
       <c r="F114" s="2">
         <f>SUM(F3:F113)</f>
-        <v>287</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -4235,8 +4253,8 @@
   <dimension ref="A1:V95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H67" sqref="H67:H200"/>
+      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S74" sqref="S74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4254,98 +4272,98 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="35" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="R2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="31" t="s">
+      <c r="S2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="V2" s="31" t="s">
+      <c r="V2" s="32" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="str">
@@ -4827,9 +4845,8 @@
         <f>IF(Aufwandsplan!D13&lt;&gt;0, Aufwandsplan!D13, "")</f>
         <v>4</v>
       </c>
-      <c r="F14" s="22" t="str">
-        <f>IF(Aufwandsplan!E13&lt;&gt;0, Aufwandsplan!E13, "")</f>
-        <v/>
+      <c r="F14" s="22">
+        <v>4</v>
       </c>
       <c r="G14" s="24">
         <f>IF(Aufwandsplan!F13&lt;&gt;0, Aufwandsplan!F13, "")</f>
@@ -4846,7 +4863,9 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
+      <c r="S14" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
@@ -6561,13 +6580,13 @@
         <f>IF(Aufwandsplan!D51&lt;&gt;0, Aufwandsplan!D51, "")</f>
         <v/>
       </c>
-      <c r="F52" s="22" t="str">
+      <c r="F52" s="22">
         <f>IF(Aufwandsplan!E51&lt;&gt;0, Aufwandsplan!E51, "")</f>
-        <v/>
-      </c>
-      <c r="G52" s="24" t="str">
+        <v>3</v>
+      </c>
+      <c r="G52" s="24">
         <f>IF(Aufwandsplan!F51&lt;&gt;0, Aufwandsplan!F51, "")</f>
-        <v/>
+        <v>-3</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="1"/>
@@ -6607,13 +6626,13 @@
         <f>IF(Aufwandsplan!D52&lt;&gt;0, Aufwandsplan!D52, "")</f>
         <v/>
       </c>
-      <c r="F53" s="22" t="str">
+      <c r="F53" s="22">
         <f>IF(Aufwandsplan!E52&lt;&gt;0, Aufwandsplan!E52, "")</f>
-        <v/>
-      </c>
-      <c r="G53" s="24" t="str">
+        <v>3</v>
+      </c>
+      <c r="G53" s="24">
         <f>IF(Aufwandsplan!F52&lt;&gt;0, Aufwandsplan!F52, "")</f>
-        <v/>
+        <v>-3</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="1"/>
@@ -6652,13 +6671,13 @@
         <f>IF(Aufwandsplan!D53&lt;&gt;0, Aufwandsplan!D53, "")</f>
         <v/>
       </c>
-      <c r="F54" s="22" t="str">
+      <c r="F54" s="22">
         <f>IF(Aufwandsplan!E53&lt;&gt;0, Aufwandsplan!E53, "")</f>
-        <v/>
-      </c>
-      <c r="G54" s="24" t="str">
+        <v>3</v>
+      </c>
+      <c r="G54" s="24">
         <f>IF(Aufwandsplan!F53&lt;&gt;0, Aufwandsplan!F53, "")</f>
-        <v/>
+        <v>-3</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="1"/>
@@ -6790,7 +6809,8 @@
         <v>8</v>
       </c>
       <c r="F57" s="22">
-        <v>12</v>
+        <f>IF(Aufwandsplan!E56&lt;&gt;0, Aufwandsplan!E56, "")</f>
+        <v>8</v>
       </c>
       <c r="G57" s="24" t="str">
         <f>IF(Aufwandsplan!F56&lt;&gt;0, Aufwandsplan!F56, "")</f>
@@ -6834,8 +6854,9 @@
         <f>IF(Aufwandsplan!D57&lt;&gt;0, Aufwandsplan!D57, "")</f>
         <v>8</v>
       </c>
-      <c r="F58" s="22">
-        <v>13</v>
+      <c r="F58" s="22" t="str">
+        <f>IF(Aufwandsplan!E57&lt;&gt;0, Aufwandsplan!E57, "")</f>
+        <v/>
       </c>
       <c r="G58" s="24">
         <f>IF(Aufwandsplan!F57&lt;&gt;0, Aufwandsplan!F57, "")</f>
@@ -7061,13 +7082,13 @@
         <f>IF(Aufwandsplan!D62&lt;&gt;0, Aufwandsplan!D62, "")</f>
         <v>12</v>
       </c>
-      <c r="F63" s="22" t="str">
+      <c r="F63" s="22">
         <f>IF(Aufwandsplan!E62&lt;&gt;0, Aufwandsplan!E62, "")</f>
-        <v/>
-      </c>
-      <c r="G63" s="24">
+        <v>12</v>
+      </c>
+      <c r="G63" s="24" t="str">
         <f>IF(Aufwandsplan!F62&lt;&gt;0, Aufwandsplan!F62, "")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="1"/>
@@ -7107,13 +7128,13 @@
         <f>IF(Aufwandsplan!D63&lt;&gt;0, Aufwandsplan!D63, "")</f>
         <v>12</v>
       </c>
-      <c r="F64" s="22" t="str">
+      <c r="F64" s="22">
         <f>IF(Aufwandsplan!E63&lt;&gt;0, Aufwandsplan!E63, "")</f>
-        <v/>
-      </c>
-      <c r="G64" s="24">
+        <v>12</v>
+      </c>
+      <c r="G64" s="24" t="str">
         <f>IF(Aufwandsplan!F63&lt;&gt;0, Aufwandsplan!F63, "")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="1"/>
@@ -7153,13 +7174,13 @@
         <f>IF(Aufwandsplan!D64&lt;&gt;0, Aufwandsplan!D64, "")</f>
         <v>12</v>
       </c>
-      <c r="F65" s="22" t="str">
+      <c r="F65" s="22">
         <f>IF(Aufwandsplan!E64&lt;&gt;0, Aufwandsplan!E64, "")</f>
-        <v/>
-      </c>
-      <c r="G65" s="24">
+        <v>12</v>
+      </c>
+      <c r="G65" s="24" t="str">
         <f>IF(Aufwandsplan!F64&lt;&gt;0, Aufwandsplan!F64, "")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="1"/>
@@ -7199,13 +7220,13 @@
         <f>IF(Aufwandsplan!D65&lt;&gt;0, Aufwandsplan!D65, "")</f>
         <v>12</v>
       </c>
-      <c r="F66" s="22" t="str">
+      <c r="F66" s="22">
         <f>IF(Aufwandsplan!E65&lt;&gt;0, Aufwandsplan!E65, "")</f>
-        <v/>
-      </c>
-      <c r="G66" s="24">
+        <v>12</v>
+      </c>
+      <c r="G66" s="24" t="str">
         <f>IF(Aufwandsplan!F65&lt;&gt;0, Aufwandsplan!F65, "")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="H66" s="7"/>
       <c r="I66" s="1"/>
@@ -7245,13 +7266,13 @@
         <f>IF(Aufwandsplan!D66&lt;&gt;0, Aufwandsplan!D66, "")</f>
         <v>12</v>
       </c>
-      <c r="F67" s="22" t="str">
+      <c r="F67" s="22">
         <f>IF(Aufwandsplan!E66&lt;&gt;0, Aufwandsplan!E66, "")</f>
-        <v/>
-      </c>
-      <c r="G67" s="24">
+        <v>12</v>
+      </c>
+      <c r="G67" s="24" t="str">
         <f>IF(Aufwandsplan!F66&lt;&gt;0, Aufwandsplan!F66, "")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="H67" s="7"/>
       <c r="I67" s="1"/>
@@ -7291,13 +7312,13 @@
         <f>IF(Aufwandsplan!D67&lt;&gt;0, Aufwandsplan!D67, "")</f>
         <v>12</v>
       </c>
-      <c r="F68" s="22" t="str">
+      <c r="F68" s="22">
         <f>IF(Aufwandsplan!E67&lt;&gt;0, Aufwandsplan!E67, "")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G68" s="24">
         <f>IF(Aufwandsplan!F67&lt;&gt;0, Aufwandsplan!F67, "")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H68" s="7"/>
       <c r="I68" s="1"/>
@@ -7431,11 +7452,11 @@
       </c>
       <c r="F71" s="22">
         <f>IF(Aufwandsplan!E70&lt;&gt;0, Aufwandsplan!E70, "")</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G71" s="24">
         <f>IF(Aufwandsplan!F70&lt;&gt;0, Aufwandsplan!F70, "")</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="1"/>
@@ -7588,7 +7609,9 @@
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
+      <c r="U74" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="V74" s="1"/>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
@@ -7632,7 +7655,9 @@
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
+      <c r="U75" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="V75" s="1"/>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -7676,7 +7701,9 @@
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
-      <c r="U76" s="1"/>
+      <c r="U76" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="V76" s="1"/>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
@@ -7719,7 +7746,9 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
       <c r="T77" s="1"/>
-      <c r="U77" s="1"/>
+      <c r="U77" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="V77" s="1"/>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
@@ -8026,7 +8055,9 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
-      <c r="T84" s="1"/>
+      <c r="T84" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
     </row>
@@ -8050,9 +8081,8 @@
         <f>IF(Aufwandsplan!D84&lt;&gt;0, Aufwandsplan!D84, "")</f>
         <v>25</v>
       </c>
-      <c r="F85" s="22" t="str">
-        <f>IF(Aufwandsplan!E84&lt;&gt;0, Aufwandsplan!E84, "")</f>
-        <v/>
+      <c r="F85" s="22">
+        <v>12</v>
       </c>
       <c r="G85" s="24">
         <f>IF(Aufwandsplan!F84&lt;&gt;0, Aufwandsplan!F84, "")</f>
@@ -8069,8 +8099,12 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
-      <c r="S85" s="1"/>
-      <c r="T85" s="1"/>
+      <c r="S85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T85" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
     </row>
@@ -8314,7 +8348,7 @@
       </c>
       <c r="U91" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V91" s="7">
         <f t="shared" si="0"/>
@@ -8378,7 +8412,7 @@
       </c>
       <c r="T92" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U92" s="7">
         <f t="shared" si="1"/>
@@ -8439,7 +8473,7 @@
       </c>
       <c r="S93" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T93" s="7">
         <f t="shared" si="2"/>
@@ -8447,7 +8481,7 @@
       </c>
       <c r="U93" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V93" s="7">
         <f t="shared" si="2"/>
@@ -8512,7 +8546,7 @@
       </c>
       <c r="U94" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V94" s="7">
         <f t="shared" si="3"/>
@@ -8569,11 +8603,11 @@
       </c>
       <c r="S95" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T95" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U95" s="7">
         <f t="shared" si="4"/>
@@ -8643,60 +8677,60 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="36" t="s">
+      <c r="J2" s="40"/>
+      <c r="K2" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
Liste offener Punkte gefüllt
</commit_message>
<xml_diff>
--- a/Doku/Managementplaene_und_listen.xlsx
+++ b/Doku/Managementplaene_und_listen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="90" windowWidth="13290" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="-30" yWindow="90" windowWidth="13290" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Strukturplan" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="379">
   <si>
     <t>Risikoliste</t>
   </si>
@@ -656,9 +656,6 @@
     <t>Mittel</t>
   </si>
   <si>
-    <t>Mit Herrn Dallmöller gesprochen. Spezifikationen festgelegt.</t>
-  </si>
-  <si>
     <t>Wie lösen wir das Vernetzungproblem?</t>
   </si>
   <si>
@@ -999,6 +996,178 @@
   </si>
   <si>
     <t>KW2</t>
+  </si>
+  <si>
+    <t>Qualitätsziele</t>
+  </si>
+  <si>
+    <t>Weche Kriterien braucht es um die Ziele zu erreichen?</t>
+  </si>
+  <si>
+    <t>Brainstorming und Diskussion -&gt; Ergebnisse an MW</t>
+  </si>
+  <si>
+    <t>Risiken</t>
+  </si>
+  <si>
+    <t>Was für Risiken sehen wir uns ausgesetzt?</t>
+  </si>
+  <si>
+    <t>Brainstorming und Diskussion -&gt; Ergebnisse an SW</t>
+  </si>
+  <si>
+    <t>Aufgaben/Arbeitspakete</t>
+  </si>
+  <si>
+    <t>Welche Aufgabe bzw. Arbeitspakete fallen an?
+Was sind die Meilensteine?</t>
+  </si>
+  <si>
+    <t>Aufwands-, Termin und Meilensteinplan</t>
+  </si>
+  <si>
+    <t>Geschäftsanwendungsfälle</t>
+  </si>
+  <si>
+    <t>siehe Anforderungen</t>
+  </si>
+  <si>
+    <t>Anforderungenvon JNK richtig?</t>
+  </si>
+  <si>
+    <t>Mit Herrn Dallmöller gesprochen. Spezifikationen festgelegt. Beantragt</t>
+  </si>
+  <si>
+    <t>Niedrig</t>
+  </si>
+  <si>
+    <t>siehe EAP-Datei</t>
+  </si>
+  <si>
+    <t>EAP</t>
+  </si>
+  <si>
+    <t>ERM gut so? Anforderungn digitalisieren in EAP</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>GUI Entwurf Eingabe Zeiten</t>
+  </si>
+  <si>
+    <t>Entwurf zusammen erarbeitet</t>
+  </si>
+  <si>
+    <t>GUI-Entwürfe digitalisieren</t>
+  </si>
+  <si>
+    <t>EA-Modell</t>
+  </si>
+  <si>
+    <t>Hinweise zu EA-Modell korrekt?</t>
+  </si>
+  <si>
+    <t>siehe Entwürfe in EAP</t>
+  </si>
+  <si>
+    <t>Präsi 1</t>
+  </si>
+  <si>
+    <t>Präsentattion so korrekt und gut?</t>
+  </si>
+  <si>
+    <t>Änderungen in Präsi1 vorgenommen</t>
+  </si>
+  <si>
+    <t>Arbeitsweise MU</t>
+  </si>
+  <si>
+    <t>Was ist zu tun um Ergebnisse von Teammitglied MU zu steigern?</t>
+  </si>
+  <si>
+    <t>Mail an MU</t>
+  </si>
+  <si>
+    <t>Wer installiert die Oracle-DB?</t>
+  </si>
+  <si>
+    <t>Oracle-DB auf Server installiert</t>
+  </si>
+  <si>
+    <t>Wer schreibt die SQL-Befehle zum Erstellen der Tabellen?</t>
+  </si>
+  <si>
+    <t>siehe sql.txt-Datei</t>
+  </si>
+  <si>
+    <t>Klassenmodell</t>
+  </si>
+  <si>
+    <t>Fehlen dort nicht die Verwaltungsklassen?</t>
+  </si>
+  <si>
+    <t>Verwaltungsklassen im Modell hinzugefügt</t>
+  </si>
+  <si>
+    <t>Wer digitalisiert das Modell</t>
+  </si>
+  <si>
+    <t>Dialoge</t>
+  </si>
+  <si>
+    <t>Diagloge müssen noch in EAP erstellt und beschrieben werden</t>
+  </si>
+  <si>
+    <t>Modell ist in EAP digitalisiert</t>
+  </si>
+  <si>
+    <t>Dialoge samt textueller Beschreibung in EA</t>
+  </si>
+  <si>
+    <t>Stundenplanerstellung</t>
+  </si>
+  <si>
+    <t>Algorithmus ist noch unbekannt. Informieren!</t>
+  </si>
+  <si>
+    <t>Algorithmus muss ofrmalisiert werden(lineares Optimierungproblem)</t>
+  </si>
+  <si>
+    <t>SQL-Befahle so korrekt(Oracle konform?)</t>
+  </si>
+  <si>
+    <t>Script zu Oracle-SQL angepasst</t>
+  </si>
+  <si>
+    <t>DB ist gefüllt</t>
+  </si>
+  <si>
+    <t>Wer erstellt die Inserts mit Daten zweier Studiengänge?</t>
+  </si>
+  <si>
+    <t>Zugriff Server</t>
+  </si>
+  <si>
+    <t>Ports zur DB und Gui müssen noch freigeschaltetw erden</t>
+  </si>
+  <si>
+    <t>Ports sind von Herrn Schulte freigeschaltet worden. Firewall angepasst</t>
+  </si>
+  <si>
+    <t>Trigger erstellt und hinzugefügt</t>
+  </si>
+  <si>
+    <t>Ist Trigger für Tabelle Zeitpräferenzen sinnvoll?</t>
+  </si>
+  <si>
+    <t>Wie formalisiert man den Algorithmus?</t>
+  </si>
+  <si>
+    <t>Wie funktioniert die Optimierung</t>
+  </si>
+  <si>
+    <t>Struktogramm Urplanerstellung</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1376,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1280,6 +1449,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
@@ -1694,7 +1865,7 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1916,7 +2087,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +2097,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1936,7 +2107,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,7 +2117,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +2137,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,96 +2147,96 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,7 +2258,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2268,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2107,7 +2278,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,7 +2330,7 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2169,7 +2340,7 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,7 +2350,7 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,7 +2360,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,7 +2370,7 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,86 +2380,86 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,7 +2479,7 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2318,7 +2489,7 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,7 +2499,7 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2349,7 +2520,7 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D75" s="1"/>
     </row>
@@ -2534,7 +2705,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" s="1">
         <v>6</v>
@@ -2908,7 +3079,7 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D32" s="1">
         <v>4</v>
@@ -2927,7 +3098,7 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
@@ -2946,7 +3117,7 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D34" s="1">
         <v>4</v>
@@ -2965,7 +3136,7 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D35" s="1">
         <v>4</v>
@@ -2996,7 +3167,7 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
@@ -3015,7 +3186,7 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
@@ -3030,11 +3201,11 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
@@ -3049,11 +3220,11 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
@@ -3068,11 +3239,11 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
@@ -3087,11 +3258,11 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D42" s="1">
         <v>10</v>
@@ -3106,11 +3277,11 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D43" s="1">
         <v>10</v>
@@ -3123,11 +3294,11 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
@@ -3142,11 +3313,11 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
@@ -3161,11 +3332,11 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
@@ -3180,11 +3351,11 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1">
@@ -3197,11 +3368,11 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1">
@@ -3214,11 +3385,11 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1">
@@ -3231,11 +3402,11 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1">
@@ -3248,11 +3419,11 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1">
@@ -3265,11 +3436,11 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1">
@@ -3282,11 +3453,11 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1">
@@ -3315,7 +3486,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D55" s="1">
         <v>8</v>
@@ -3334,7 +3505,7 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D56" s="1">
         <v>8</v>
@@ -3353,7 +3524,7 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D57" s="1">
         <v>8</v>
@@ -3432,7 +3603,7 @@
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D62" s="1">
         <v>12</v>
@@ -3451,7 +3622,7 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D63" s="1">
         <v>12</v>
@@ -3470,7 +3641,7 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D64" s="1">
         <v>12</v>
@@ -3489,7 +3660,7 @@
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D65" s="1">
         <v>12</v>
@@ -3508,7 +3679,7 @@
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D66" s="1">
         <v>12</v>
@@ -3527,7 +3698,7 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D67" s="1">
         <v>12</v>
@@ -3542,11 +3713,11 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D68" s="1">
         <v>12</v>
@@ -3559,11 +3730,11 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D69" s="1">
         <v>12</v>
@@ -3576,11 +3747,11 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D70" s="1">
         <v>22</v>
@@ -3595,11 +3766,11 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D71" s="1">
         <v>22</v>
@@ -3612,11 +3783,11 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D72" s="1">
         <v>12</v>
@@ -3629,11 +3800,11 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D73" s="1">
         <v>12</v>
@@ -3646,11 +3817,11 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D74" s="1">
         <v>12</v>
@@ -3663,11 +3834,11 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3678,11 +3849,11 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -3693,11 +3864,11 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3708,11 +3879,11 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3723,11 +3894,11 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3738,11 +3909,11 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -3753,11 +3924,11 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -3787,7 +3958,7 @@
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D83" s="1">
         <v>25</v>
@@ -3804,7 +3975,7 @@
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D84" s="1">
         <v>25</v>
@@ -3821,7 +3992,7 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D85" s="1">
         <v>25</v>
@@ -3854,7 +4025,7 @@
         <v>170</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1">
@@ -4084,7 +4255,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C114" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D114" s="2">
         <f>SUM(D3:D113)</f>
@@ -4146,7 +4317,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
@@ -4163,7 +4334,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -4180,7 +4351,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>47</v>
@@ -4197,7 +4368,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>48</v>
@@ -4214,10 +4385,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>216</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>217</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
@@ -4252,7 +4423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S74" sqref="S74"/>
     </sheetView>
@@ -4333,10 +4504,10 @@
         <v>36</v>
       </c>
       <c r="U2" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="V2" s="32" t="s">
         <v>321</v>
-      </c>
-      <c r="V2" s="32" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4864,7 +5035,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -5305,7 +5476,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -5352,7 +5523,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -5399,7 +5570,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -5444,7 +5615,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -5580,7 +5751,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -5763,7 +5934,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -5809,7 +5980,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -5856,7 +6027,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -6127,10 +6298,10 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -6413,7 +6584,7 @@
         <v>116</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="28"/>
@@ -6460,7 +6631,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
@@ -6506,7 +6677,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
@@ -6552,7 +6723,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -6599,7 +6770,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -6644,7 +6815,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="R53" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -6690,7 +6861,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S54" s="28"/>
       <c r="T54" s="1"/>
@@ -7286,7 +7457,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -7563,7 +7734,7 @@
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
@@ -7610,7 +7781,7 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V74" s="1"/>
     </row>
@@ -8286,10 +8457,10 @@
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B91" s="27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G91" s="9" t="s">
         <v>87</v>
@@ -8357,7 +8528,7 @@
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B92" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G92" s="9" t="s">
         <v>89</v>
@@ -8425,7 +8596,7 @@
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G93" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H93" s="7">
         <f>COUNTIF(H4:H89,"JNK")+COUNTIF(H4:H89,"alle")</f>
@@ -8649,17 +8820,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
@@ -8668,7 +8839,7 @@
     <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
@@ -8740,7 +8911,7 @@
         <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>115</v>
@@ -8781,7 +8952,7 @@
         <v>120</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>207</v>
+        <v>335</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>121</v>
@@ -8793,7 +8964,7 @@
         <v>121</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>121</v>
@@ -8801,7 +8972,9 @@
       <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="L5" s="1" t="s">
         <v>122</v>
       </c>
@@ -8814,348 +8987,868 @@
         <v>206</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>90</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>117</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>208</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="A28" s="43">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -9167,8 +9860,8 @@
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -9193,6 +9886,34 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -9216,7 +9937,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9246,10 +9967,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
@@ -9378,7 +10099,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>98</v>
@@ -9531,7 +10252,7 @@
         <v>90</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Liste offener Punkte DONE
</commit_message>
<xml_diff>
--- a/Doku/Managementplaene_und_listen.xlsx
+++ b/Doku/Managementplaene_und_listen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="412">
   <si>
     <t>Risikoliste</t>
   </si>
@@ -1168,13 +1168,112 @@
   </si>
   <si>
     <t>Struktogramm Urplanerstellung</t>
+  </si>
+  <si>
+    <t>Spezifikation Testdurchführung</t>
+  </si>
+  <si>
+    <t>KW02</t>
+  </si>
+  <si>
+    <t>Dokument wurde im Git hinzugefügt. Absprache mit MU</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Durchführung Test</t>
+  </si>
+  <si>
+    <t>KW04</t>
+  </si>
+  <si>
+    <t>siehe Dokument</t>
+  </si>
+  <si>
+    <t>bis auf weiteres ausgesetzt</t>
+  </si>
+  <si>
+    <t>KW03</t>
+  </si>
+  <si>
+    <t>KW05</t>
+  </si>
+  <si>
+    <t>siehe Dokument (unter "Weitere_Dokumente")</t>
+  </si>
+  <si>
+    <t>Abschlusspräsentation erstellen</t>
+  </si>
+  <si>
+    <t>siehe PPTX</t>
+  </si>
+  <si>
+    <t>Präsi 3</t>
+  </si>
+  <si>
+    <t>Dokumentation Fortschritt der Optimierung</t>
+  </si>
+  <si>
+    <t>Dokument zur Aufgabenstellung und Möglichkeiten</t>
+  </si>
+  <si>
+    <t>Niedirg</t>
+  </si>
+  <si>
+    <t>Programmierung</t>
+  </si>
+  <si>
+    <t>Problem Seitenreload  Urplanersellung beheben</t>
+  </si>
+  <si>
+    <t>siehe Programm</t>
+  </si>
+  <si>
+    <t>Installation JBOSS Standalone</t>
+  </si>
+  <si>
+    <t>MW/SW</t>
+  </si>
+  <si>
+    <t>Server installiert</t>
+  </si>
+  <si>
+    <t>Formatierung Dokumente  vereinheitlichen</t>
+  </si>
+  <si>
+    <t>siehe Dokumente (unter "Weitere_Dokumente")</t>
+  </si>
+  <si>
+    <t>Anpassung der Präsentation</t>
+  </si>
+  <si>
+    <t>siehe Präsentation</t>
+  </si>
+  <si>
+    <t>Überprüfung der abzugebeden Dokumente</t>
+  </si>
+  <si>
+    <t>Dokumente geprüft, sortiert und Liste an JNK geschickt</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
+  </si>
+  <si>
+    <t>Sammeln der Dateien in Dropbox</t>
+  </si>
+  <si>
+    <t>alle/JNK</t>
+  </si>
+  <si>
+    <t>Alle Dokumente befinden sich im Dropbox-Ordner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1200,6 +1299,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1376,7 +1483,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1419,6 +1526,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1449,8 +1558,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
@@ -4443,98 +4551,98 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="37" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="32" t="s">
+      <c r="R2" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="T2" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="U2" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="34" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="36"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="str">
@@ -8791,15 +8899,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -8812,6 +8911,15 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8820,10 +8928,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8848,60 +8956,60 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="37" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="37" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="40" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -8955,7 +9063,7 @@
         <v>335</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>26</v>
@@ -9221,7 +9329,7 @@
         <v>207</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>28</v>
@@ -9259,7 +9367,7 @@
         <v>207</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>29</v>
@@ -9691,7 +9799,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="44" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -9745,7 +9855,7 @@
         <v>115</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>34</v>
@@ -9808,7 +9918,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="33">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -9846,74 +9956,422 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="A30" s="32">
+        <v>27</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <v>31</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>397</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="J34" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="K34" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L34" s="33" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="33">
+        <v>32</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="K35" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L35" s="33" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <v>33</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="K36" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="33">
+        <v>34</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="K37" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" s="33" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <v>35</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>406</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="K38" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L38" s="33" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>36</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>410</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="J39" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="K39" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L39" s="33" t="s">
+        <v>411</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -9929,6 +10387,7 @@
     <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Termin- und Meilensteinplan DONE
</commit_message>
<xml_diff>
--- a/Doku/Managementplaene_und_listen.xlsx
+++ b/Doku/Managementplaene_und_listen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="90" windowWidth="13290" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-30" yWindow="90" windowWidth="13290" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Strukturplan" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="403">
   <si>
     <t>Risikoliste</t>
   </si>
@@ -1456,7 +1456,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1531,6 +1531,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
@@ -2761,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,11 +2961,11 @@
         <v>4</v>
       </c>
       <c r="E12" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3504,11 +3506,11 @@
         <v>15</v>
       </c>
       <c r="E43" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="0"/>
-        <v>-12</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3870,11 +3872,11 @@
         <v>20</v>
       </c>
       <c r="E64" s="1">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="0"/>
-        <v>-23</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3927,11 +3929,11 @@
         <v>12</v>
       </c>
       <c r="E67" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -4020,11 +4022,11 @@
         <v>22</v>
       </c>
       <c r="E72" s="1">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="0"/>
-        <v>-35</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -4056,11 +4058,11 @@
         <v>12</v>
       </c>
       <c r="E74" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -4092,11 +4094,11 @@
         <v>12</v>
       </c>
       <c r="E76" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -4109,11 +4111,11 @@
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="0"/>
-        <v>-15</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -4126,11 +4128,11 @@
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F78" s="1">
         <f t="shared" si="0"/>
-        <v>-12</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -4143,11 +4145,11 @@
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F79" s="1">
         <f t="shared" si="0"/>
-        <v>-15</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -4217,11 +4219,11 @@
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -4234,10 +4236,7 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -4289,11 +4288,11 @@
         <v>25</v>
       </c>
       <c r="E87" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4562,11 +4561,11 @@
       </c>
       <c r="E116" s="2">
         <f>SUM(E3:E115)</f>
-        <v>688</v>
+        <v>626</v>
       </c>
       <c r="F116" s="2">
         <f>SUM(F3:F115)</f>
-        <v>-168</v>
+        <v>-106</v>
       </c>
     </row>
   </sheetData>
@@ -4720,11 +4719,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y101"/>
+  <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
+      <selection pane="bottomLeft" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4732,7 +4731,7 @@
     <col min="1" max="1" width="8.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.42578125" style="21" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
@@ -4871,7 +4870,7 @@
         <f>IF(Aufwandsplan!E3&lt;&gt;0, Aufwandsplan!E3, "")</f>
         <v/>
       </c>
-      <c r="G4" s="22" t="str">
+      <c r="G4" s="44" t="str">
         <f>IF(Aufwandsplan!F3&lt;&gt;0, Aufwandsplan!F3, "")</f>
         <v/>
       </c>
@@ -4916,7 +4915,7 @@
         <f>IF(Aufwandsplan!E4&lt;&gt;0, Aufwandsplan!E4, "")</f>
         <v>2</v>
       </c>
-      <c r="G5" s="22" t="str">
+      <c r="G5" s="44" t="str">
         <f>IF(Aufwandsplan!F4&lt;&gt;0, Aufwandsplan!F4, "")</f>
         <v/>
       </c>
@@ -4963,7 +4962,7 @@
         <f>IF(Aufwandsplan!E5&lt;&gt;0, Aufwandsplan!E5, "")</f>
         <v>2</v>
       </c>
-      <c r="G6" s="22" t="str">
+      <c r="G6" s="44" t="str">
         <f>IF(Aufwandsplan!F5&lt;&gt;0, Aufwandsplan!F5, "")</f>
         <v/>
       </c>
@@ -5010,7 +5009,7 @@
         <f>IF(Aufwandsplan!E6&lt;&gt;0, Aufwandsplan!E6, "")</f>
         <v>2</v>
       </c>
-      <c r="G7" s="22" t="str">
+      <c r="G7" s="44" t="str">
         <f>IF(Aufwandsplan!F6&lt;&gt;0, Aufwandsplan!F6, "")</f>
         <v/>
       </c>
@@ -5057,7 +5056,7 @@
         <f>IF(Aufwandsplan!E7&lt;&gt;0, Aufwandsplan!E7, "")</f>
         <v/>
       </c>
-      <c r="G8" s="22" t="str">
+      <c r="G8" s="44" t="str">
         <f>IF(Aufwandsplan!F7&lt;&gt;0, Aufwandsplan!F7, "")</f>
         <v/>
       </c>
@@ -5102,7 +5101,7 @@
         <f>IF(Aufwandsplan!E8&lt;&gt;0, Aufwandsplan!E8, "")</f>
         <v>8</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="44">
         <f>IF(Aufwandsplan!F8&lt;&gt;0, Aufwandsplan!F8, "")</f>
         <v>-2</v>
       </c>
@@ -5151,7 +5150,7 @@
         <f>IF(Aufwandsplan!E9&lt;&gt;0, Aufwandsplan!E9, "")</f>
         <v>5</v>
       </c>
-      <c r="G10" s="22" t="str">
+      <c r="G10" s="44" t="str">
         <f>IF(Aufwandsplan!F9&lt;&gt;0, Aufwandsplan!F9, "")</f>
         <v/>
       </c>
@@ -5198,7 +5197,7 @@
         <f>IF(Aufwandsplan!E10&lt;&gt;0, Aufwandsplan!E10, "")</f>
         <v>11</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="44">
         <f>IF(Aufwandsplan!F10&lt;&gt;0, Aufwandsplan!F10, "")</f>
         <v>-5</v>
       </c>
@@ -5245,7 +5244,7 @@
         <f>IF(Aufwandsplan!E11&lt;&gt;0, Aufwandsplan!E11, "")</f>
         <v/>
       </c>
-      <c r="G12" s="22" t="str">
+      <c r="G12" s="44" t="str">
         <f>IF(Aufwandsplan!F11&lt;&gt;0, Aufwandsplan!F11, "")</f>
         <v/>
       </c>
@@ -5288,11 +5287,11 @@
       </c>
       <c r="F13" s="22">
         <f>IF(Aufwandsplan!E12&lt;&gt;0, Aufwandsplan!E12, "")</f>
-        <v>4</v>
-      </c>
-      <c r="G13" s="22" t="str">
+        <v>6</v>
+      </c>
+      <c r="G13" s="44">
         <f>IF(Aufwandsplan!F12&lt;&gt;0, Aufwandsplan!F12, "")</f>
-        <v/>
+        <v>-2</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
@@ -5341,7 +5340,7 @@
         <f>IF(Aufwandsplan!E13&lt;&gt;0, Aufwandsplan!E13, "")</f>
         <v>4</v>
       </c>
-      <c r="G14" s="22" t="str">
+      <c r="G14" s="44" t="str">
         <f>IF(Aufwandsplan!F13&lt;&gt;0, Aufwandsplan!F13, "")</f>
         <v/>
       </c>
@@ -5388,7 +5387,7 @@
         <f>IF(Aufwandsplan!E14&lt;&gt;0, Aufwandsplan!E14, "")</f>
         <v>12</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="44">
         <f>IF(Aufwandsplan!F14&lt;&gt;0, Aufwandsplan!F14, "")</f>
         <v>-8</v>
       </c>
@@ -5441,7 +5440,7 @@
         <f>IF(Aufwandsplan!E15&lt;&gt;0, Aufwandsplan!E15, "")</f>
         <v/>
       </c>
-      <c r="G16" s="22" t="str">
+      <c r="G16" s="44" t="str">
         <f>IF(Aufwandsplan!F15&lt;&gt;0, Aufwandsplan!F15, "")</f>
         <v/>
       </c>
@@ -5486,7 +5485,7 @@
         <f>IF(Aufwandsplan!E16&lt;&gt;0, Aufwandsplan!E16, "")</f>
         <v>5</v>
       </c>
-      <c r="G17" s="22" t="str">
+      <c r="G17" s="44" t="str">
         <f>IF(Aufwandsplan!F16&lt;&gt;0, Aufwandsplan!F16, "")</f>
         <v/>
       </c>
@@ -5533,7 +5532,7 @@
         <f>IF(Aufwandsplan!E17&lt;&gt;0, Aufwandsplan!E17, "")</f>
         <v>5</v>
       </c>
-      <c r="G18" s="22" t="str">
+      <c r="G18" s="44" t="str">
         <f>IF(Aufwandsplan!F17&lt;&gt;0, Aufwandsplan!F17, "")</f>
         <v/>
       </c>
@@ -5582,7 +5581,7 @@
         <f>IF(Aufwandsplan!E18&lt;&gt;0, Aufwandsplan!E18, "")</f>
         <v>8</v>
       </c>
-      <c r="G19" s="22" t="str">
+      <c r="G19" s="44" t="str">
         <f>IF(Aufwandsplan!F18&lt;&gt;0, Aufwandsplan!F18, "")</f>
         <v/>
       </c>
@@ -5629,7 +5628,7 @@
         <f>IF(Aufwandsplan!E19&lt;&gt;0, Aufwandsplan!E19, "")</f>
         <v/>
       </c>
-      <c r="G20" s="22" t="str">
+      <c r="G20" s="44" t="str">
         <f>IF(Aufwandsplan!F19&lt;&gt;0, Aufwandsplan!F19, "")</f>
         <v/>
       </c>
@@ -5674,7 +5673,7 @@
         <f>IF(Aufwandsplan!E20&lt;&gt;0, Aufwandsplan!E20, "")</f>
         <v>10</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="44">
         <f>IF(Aufwandsplan!F20&lt;&gt;0, Aufwandsplan!F20, "")</f>
         <v>-4</v>
       </c>
@@ -5719,7 +5718,7 @@
         <f>IF(Aufwandsplan!E21&lt;&gt;0, Aufwandsplan!E21, "")</f>
         <v>8</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="44">
         <f>IF(Aufwandsplan!F21&lt;&gt;0, Aufwandsplan!F21, "")</f>
         <v>2</v>
       </c>
@@ -5766,7 +5765,7 @@
         <f>IF(Aufwandsplan!E22&lt;&gt;0, Aufwandsplan!E22, "")</f>
         <v/>
       </c>
-      <c r="G23" s="22" t="str">
+      <c r="G23" s="44" t="str">
         <f>IF(Aufwandsplan!F22&lt;&gt;0, Aufwandsplan!F22, "")</f>
         <v/>
       </c>
@@ -5811,7 +5810,7 @@
         <f>IF(Aufwandsplan!E23&lt;&gt;0, Aufwandsplan!E23, "")</f>
         <v>10</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="44">
         <f>IF(Aufwandsplan!F23&lt;&gt;0, Aufwandsplan!F23, "")</f>
         <v>-2</v>
       </c>
@@ -5858,7 +5857,7 @@
         <f>IF(Aufwandsplan!E24&lt;&gt;0, Aufwandsplan!E24, "")</f>
         <v>6</v>
       </c>
-      <c r="G25" s="22" t="str">
+      <c r="G25" s="44" t="str">
         <f>IF(Aufwandsplan!F24&lt;&gt;0, Aufwandsplan!F24, "")</f>
         <v/>
       </c>
@@ -5905,7 +5904,7 @@
         <f>IF(Aufwandsplan!E25&lt;&gt;0, Aufwandsplan!E25, "")</f>
         <v>6</v>
       </c>
-      <c r="G26" s="22" t="str">
+      <c r="G26" s="44" t="str">
         <f>IF(Aufwandsplan!F25&lt;&gt;0, Aufwandsplan!F25, "")</f>
         <v/>
       </c>
@@ -5952,7 +5951,7 @@
         <f>IF(Aufwandsplan!E26&lt;&gt;0, Aufwandsplan!E26, "")</f>
         <v>2</v>
       </c>
-      <c r="G27" s="22" t="str">
+      <c r="G27" s="44" t="str">
         <f>IF(Aufwandsplan!F26&lt;&gt;0, Aufwandsplan!F26, "")</f>
         <v/>
       </c>
@@ -6001,7 +6000,7 @@
         <f>IF(Aufwandsplan!E27&lt;&gt;0, Aufwandsplan!E27, "")</f>
         <v/>
       </c>
-      <c r="G28" s="22" t="str">
+      <c r="G28" s="44" t="str">
         <f>IF(Aufwandsplan!F27&lt;&gt;0, Aufwandsplan!F27, "")</f>
         <v/>
       </c>
@@ -6013,6 +6012,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="29"/>
       <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -6045,7 +6045,7 @@
         <f>IF(Aufwandsplan!E28&lt;&gt;0, Aufwandsplan!E28, "")</f>
         <v>10</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="44">
         <f>IF(Aufwandsplan!F28&lt;&gt;0, Aufwandsplan!F28, "")</f>
         <v>-2</v>
       </c>
@@ -6092,7 +6092,7 @@
         <f>IF(Aufwandsplan!E29&lt;&gt;0, Aufwandsplan!E29, "")</f>
         <v>7</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="44">
         <f>IF(Aufwandsplan!F29&lt;&gt;0, Aufwandsplan!F29, "")</f>
         <v>-2</v>
       </c>
@@ -6139,7 +6139,7 @@
         <f>IF(Aufwandsplan!E30&lt;&gt;0, Aufwandsplan!E30, "")</f>
         <v>8</v>
       </c>
-      <c r="G31" s="22" t="str">
+      <c r="G31" s="44" t="str">
         <f>IF(Aufwandsplan!F30&lt;&gt;0, Aufwandsplan!F30, "")</f>
         <v/>
       </c>
@@ -6188,7 +6188,7 @@
         <f>IF(Aufwandsplan!E31&lt;&gt;0, Aufwandsplan!E31, "")</f>
         <v/>
       </c>
-      <c r="G32" s="22" t="str">
+      <c r="G32" s="44" t="str">
         <f>IF(Aufwandsplan!F31&lt;&gt;0, Aufwandsplan!F31, "")</f>
         <v/>
       </c>
@@ -6199,6 +6199,8 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="29"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -6231,7 +6233,7 @@
         <f>IF(Aufwandsplan!E32&lt;&gt;0, Aufwandsplan!E32, "")</f>
         <v>4</v>
       </c>
-      <c r="G33" s="22" t="str">
+      <c r="G33" s="44" t="str">
         <f>IF(Aufwandsplan!F32&lt;&gt;0, Aufwandsplan!F32, "")</f>
         <v/>
       </c>
@@ -6278,7 +6280,7 @@
         <f>IF(Aufwandsplan!E33&lt;&gt;0, Aufwandsplan!E33, "")</f>
         <v>2</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="44">
         <f>IF(Aufwandsplan!F33&lt;&gt;0, Aufwandsplan!F33, "")</f>
         <v>2</v>
       </c>
@@ -6325,7 +6327,7 @@
         <f>IF(Aufwandsplan!E34&lt;&gt;0, Aufwandsplan!E34, "")</f>
         <v>8</v>
       </c>
-      <c r="G35" s="22" t="str">
+      <c r="G35" s="44" t="str">
         <f>IF(Aufwandsplan!F34&lt;&gt;0, Aufwandsplan!F34, "")</f>
         <v/>
       </c>
@@ -6372,7 +6374,7 @@
         <f>IF(Aufwandsplan!E35&lt;&gt;0, Aufwandsplan!E35, "")</f>
         <v>4</v>
       </c>
-      <c r="G36" s="22" t="str">
+      <c r="G36" s="44" t="str">
         <f>IF(Aufwandsplan!F35&lt;&gt;0, Aufwandsplan!F35, "")</f>
         <v/>
       </c>
@@ -6419,7 +6421,7 @@
         <f>IF(Aufwandsplan!E36&lt;&gt;0, Aufwandsplan!E36, "")</f>
         <v>2</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="44">
         <f>IF(Aufwandsplan!F36&lt;&gt;0, Aufwandsplan!F36, "")</f>
         <v>-2</v>
       </c>
@@ -6429,9 +6431,12 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="P37" s="25"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="29"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -6461,7 +6466,7 @@
         <f>IF(Aufwandsplan!E37&lt;&gt;0, Aufwandsplan!E37, "")</f>
         <v/>
       </c>
-      <c r="G38" s="22" t="str">
+      <c r="G38" s="44" t="str">
         <f>IF(Aufwandsplan!F37&lt;&gt;0, Aufwandsplan!F37, "")</f>
         <v/>
       </c>
@@ -6471,13 +6476,11 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="N38" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="P38" s="25"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+      <c r="R38" s="29"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
@@ -6508,7 +6511,7 @@
         <f>IF(Aufwandsplan!E38&lt;&gt;0, Aufwandsplan!E38, "")</f>
         <v>3</v>
       </c>
-      <c r="G39" s="22" t="str">
+      <c r="G39" s="44" t="str">
         <f>IF(Aufwandsplan!F38&lt;&gt;0, Aufwandsplan!F38, "")</f>
         <v/>
       </c>
@@ -6519,7 +6522,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -6555,7 +6558,7 @@
         <f>IF(Aufwandsplan!E39&lt;&gt;0, Aufwandsplan!E39, "")</f>
         <v>3</v>
       </c>
-      <c r="G40" s="22" t="str">
+      <c r="G40" s="44" t="str">
         <f>IF(Aufwandsplan!F39&lt;&gt;0, Aufwandsplan!F39, "")</f>
         <v/>
       </c>
@@ -6566,7 +6569,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -6602,7 +6605,7 @@
         <f>IF(Aufwandsplan!E40&lt;&gt;0, Aufwandsplan!E40, "")</f>
         <v>3</v>
       </c>
-      <c r="G41" s="22" t="str">
+      <c r="G41" s="44" t="str">
         <f>IF(Aufwandsplan!F40&lt;&gt;0, Aufwandsplan!F40, "")</f>
         <v/>
       </c>
@@ -6612,10 +6615,10 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="N41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -6649,7 +6652,7 @@
         <f>IF(Aufwandsplan!E41&lt;&gt;0, Aufwandsplan!E41, "")</f>
         <v>3</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="44">
         <f>IF(Aufwandsplan!F41&lt;&gt;0, Aufwandsplan!F41, "")</f>
         <v>-3</v>
       </c>
@@ -6659,12 +6662,8 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -6698,7 +6697,7 @@
         <f>IF(Aufwandsplan!E42&lt;&gt;0, Aufwandsplan!E42, "")</f>
         <v>3</v>
       </c>
-      <c r="G43" s="22" t="str">
+      <c r="G43" s="44" t="str">
         <f>IF(Aufwandsplan!F42&lt;&gt;0, Aufwandsplan!F42, "")</f>
         <v/>
       </c>
@@ -6708,16 +6707,14 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="N43" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O43" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -6747,11 +6744,11 @@
       </c>
       <c r="F44" s="22">
         <f>IF(Aufwandsplan!E43&lt;&gt;0, Aufwandsplan!E43, "")</f>
-        <v>27</v>
-      </c>
-      <c r="G44" s="22">
+        <v>23</v>
+      </c>
+      <c r="G44" s="44">
         <f>IF(Aufwandsplan!F43&lt;&gt;0, Aufwandsplan!F43, "")</f>
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="1"/>
@@ -6761,10 +6758,14 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="27"/>
+        <v>217</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
@@ -6796,7 +6797,7 @@
         <f>IF(Aufwandsplan!E44&lt;&gt;0, Aufwandsplan!E44, "")</f>
         <v>2</v>
       </c>
-      <c r="G45" s="22">
+      <c r="G45" s="44">
         <f>IF(Aufwandsplan!F44&lt;&gt;0, Aufwandsplan!F44, "")</f>
         <v>-2</v>
       </c>
@@ -6808,7 +6809,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
@@ -6843,7 +6844,7 @@
         <f>IF(Aufwandsplan!E45&lt;&gt;0, Aufwandsplan!E45, "")</f>
         <v>3</v>
       </c>
-      <c r="G46" s="22" t="str">
+      <c r="G46" s="44" t="str">
         <f>IF(Aufwandsplan!F45&lt;&gt;0, Aufwandsplan!F45, "")</f>
         <v/>
       </c>
@@ -6853,10 +6854,10 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="N46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -6890,7 +6891,7 @@
         <f>IF(Aufwandsplan!E46&lt;&gt;0, Aufwandsplan!E46, "")</f>
         <v>3</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="44">
         <f>IF(Aufwandsplan!F46&lt;&gt;0, Aufwandsplan!F46, "")</f>
         <v>-3</v>
       </c>
@@ -6900,9 +6901,11 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+      <c r="N47" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="O47" s="1" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -6937,7 +6940,7 @@
         <f>IF(Aufwandsplan!E47&lt;&gt;0, Aufwandsplan!E47, "")</f>
         <v>3</v>
       </c>
-      <c r="G48" s="22" t="str">
+      <c r="G48" s="44" t="str">
         <f>IF(Aufwandsplan!F47&lt;&gt;0, Aufwandsplan!F47, "")</f>
         <v/>
       </c>
@@ -6948,12 +6951,8 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="27"/>
       <c r="S48" s="1"/>
@@ -6986,7 +6985,7 @@
         <f>IF(Aufwandsplan!E48&lt;&gt;0, Aufwandsplan!E48, "")</f>
         <v>3</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="44">
         <f>IF(Aufwandsplan!F48&lt;&gt;0, Aufwandsplan!F48, "")</f>
         <v>-3</v>
       </c>
@@ -6997,11 +6996,13 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1" t="s">
+      <c r="O49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P49" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -7033,7 +7034,7 @@
         <f>IF(Aufwandsplan!E49&lt;&gt;0, Aufwandsplan!E49, "")</f>
         <v>3</v>
       </c>
-      <c r="G50" s="22">
+      <c r="G50" s="44">
         <f>IF(Aufwandsplan!F49&lt;&gt;0, Aufwandsplan!F49, "")</f>
         <v>-3</v>
       </c>
@@ -7044,7 +7045,9 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
+      <c r="O50" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="P50" s="1"/>
       <c r="Q50" s="1" t="s">
         <v>217</v>
@@ -7080,7 +7083,7 @@
         <f>IF(Aufwandsplan!E50&lt;&gt;0, Aufwandsplan!E50, "")</f>
         <v>3</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="44">
         <f>IF(Aufwandsplan!F50&lt;&gt;0, Aufwandsplan!F50, "")</f>
         <v>-3</v>
       </c>
@@ -7127,7 +7130,7 @@
         <f>IF(Aufwandsplan!E51&lt;&gt;0, Aufwandsplan!E51, "")</f>
         <v>2</v>
       </c>
-      <c r="G52" s="22">
+      <c r="G52" s="44">
         <f>IF(Aufwandsplan!F51&lt;&gt;0, Aufwandsplan!F51, "")</f>
         <v>1</v>
       </c>
@@ -7140,10 +7143,10 @@
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1" t="s">
+      <c r="Q52" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
@@ -7174,7 +7177,7 @@
         <f>IF(Aufwandsplan!E52&lt;&gt;0, Aufwandsplan!E52, "")</f>
         <v>3</v>
       </c>
-      <c r="G53" s="22" t="str">
+      <c r="G53" s="44" t="str">
         <f>IF(Aufwandsplan!F52&lt;&gt;0, Aufwandsplan!F52, "")</f>
         <v/>
       </c>
@@ -7187,6 +7190,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
       <c r="R53" s="1" t="s">
         <v>217</v>
       </c>
@@ -7220,7 +7224,7 @@
         <f>IF(Aufwandsplan!E53&lt;&gt;0, Aufwandsplan!E53, "")</f>
         <v>3</v>
       </c>
-      <c r="G54" s="22" t="str">
+      <c r="G54" s="44" t="str">
         <f>IF(Aufwandsplan!F53&lt;&gt;0, Aufwandsplan!F53, "")</f>
         <v/>
       </c>
@@ -7267,7 +7271,7 @@
         <f>IF(Aufwandsplan!E54&lt;&gt;0, Aufwandsplan!E54, "")</f>
         <v>2</v>
       </c>
-      <c r="G55" s="22">
+      <c r="G55" s="44">
         <f>IF(Aufwandsplan!F54&lt;&gt;0, Aufwandsplan!F54, "")</f>
         <v>-2</v>
       </c>
@@ -7281,7 +7285,9 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
+      <c r="R55" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
@@ -7314,7 +7320,7 @@
         <f>IF(Aufwandsplan!E55&lt;&gt;0, Aufwandsplan!E55, "")</f>
         <v/>
       </c>
-      <c r="G56" s="22" t="str">
+      <c r="G56" s="44" t="str">
         <f>IF(Aufwandsplan!F55&lt;&gt;0, Aufwandsplan!F55, "")</f>
         <v/>
       </c>
@@ -7324,14 +7330,11 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="N56" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
@@ -7362,7 +7365,7 @@
         <f>IF(Aufwandsplan!E56&lt;&gt;0, Aufwandsplan!E56, "")</f>
         <v>8</v>
       </c>
-      <c r="G57" s="22" t="str">
+      <c r="G57" s="44" t="str">
         <f>IF(Aufwandsplan!F56&lt;&gt;0, Aufwandsplan!F56, "")</f>
         <v/>
       </c>
@@ -7372,11 +7375,11 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
+      <c r="N57" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="O57" s="1"/>
-      <c r="P57" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -7409,7 +7412,7 @@
         <f>IF(Aufwandsplan!E57&lt;&gt;0, Aufwandsplan!E57, "")</f>
         <v>8</v>
       </c>
-      <c r="G58" s="22" t="str">
+      <c r="G58" s="44" t="str">
         <f>IF(Aufwandsplan!F57&lt;&gt;0, Aufwandsplan!F57, "")</f>
         <v/>
       </c>
@@ -7420,8 +7423,12 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
+      <c r="O58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="Q58" s="1" t="s">
         <v>121</v>
       </c>
@@ -7458,7 +7465,7 @@
         <f>IF(Aufwandsplan!E58&lt;&gt;0, Aufwandsplan!E58, "")</f>
         <v>6</v>
       </c>
-      <c r="G59" s="22">
+      <c r="G59" s="44">
         <f>IF(Aufwandsplan!F58&lt;&gt;0, Aufwandsplan!F58, "")</f>
         <v>2</v>
       </c>
@@ -7470,8 +7477,9 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="25"/>
-      <c r="R59" s="29"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
@@ -7504,7 +7512,7 @@
         <f>IF(Aufwandsplan!E59&lt;&gt;0, Aufwandsplan!E59, "")</f>
         <v/>
       </c>
-      <c r="G60" s="22" t="str">
+      <c r="G60" s="44" t="str">
         <f>IF(Aufwandsplan!F59&lt;&gt;0, Aufwandsplan!F59, "")</f>
         <v/>
       </c>
@@ -7514,15 +7522,11 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
-      <c r="N60" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="P60" s="25"/>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
+      <c r="R60" s="29"/>
       <c r="S60" s="1"/>
       <c r="T60" s="27"/>
       <c r="U60" s="1"/>
@@ -7553,7 +7557,7 @@
         <f>IF(Aufwandsplan!E60&lt;&gt;0, Aufwandsplan!E60, "")</f>
         <v>15</v>
       </c>
-      <c r="G61" s="22" t="str">
+      <c r="G61" s="44" t="str">
         <f>IF(Aufwandsplan!F60&lt;&gt;0, Aufwandsplan!F60, "")</f>
         <v/>
       </c>
@@ -7563,9 +7567,13 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
+      <c r="N61" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
+      <c r="P61" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="Q61" s="1" t="s">
         <v>116</v>
       </c>
@@ -7600,7 +7608,7 @@
         <f>IF(Aufwandsplan!E61&lt;&gt;0, Aufwandsplan!E61, "")</f>
         <v>12</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G62" s="44">
         <f>IF(Aufwandsplan!F61&lt;&gt;0, Aufwandsplan!F61, "")</f>
         <v>22</v>
       </c>
@@ -7613,7 +7621,8 @@
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
-      <c r="R62" s="25"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
@@ -7644,7 +7653,7 @@
         <f>IF(Aufwandsplan!E62&lt;&gt;0, Aufwandsplan!E62, "")</f>
         <v/>
       </c>
-      <c r="G63" s="22" t="str">
+      <c r="G63" s="44" t="str">
         <f>IF(Aufwandsplan!F62&lt;&gt;0, Aufwandsplan!F62, "")</f>
         <v/>
       </c>
@@ -7658,15 +7667,13 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-      <c r="R63" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="R63" s="25"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
+      <c r="X63" s="29"/>
       <c r="Y63" s="1"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
@@ -7691,7 +7698,7 @@
         <f>IF(Aufwandsplan!E63&lt;&gt;0, Aufwandsplan!E63, "")</f>
         <v>12</v>
       </c>
-      <c r="G64" s="22" t="str">
+      <c r="G64" s="44" t="str">
         <f>IF(Aufwandsplan!F63&lt;&gt;0, Aufwandsplan!F63, "")</f>
         <v/>
       </c>
@@ -7706,7 +7713,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -7736,11 +7743,11 @@
       </c>
       <c r="F65" s="22">
         <f>IF(Aufwandsplan!E64&lt;&gt;0, Aufwandsplan!E64, "")</f>
-        <v>43</v>
-      </c>
-      <c r="G65" s="22">
+        <v>24</v>
+      </c>
+      <c r="G65" s="44">
         <f>IF(Aufwandsplan!F64&lt;&gt;0, Aufwandsplan!F64, "")</f>
-        <v>-23</v>
+        <v>-4</v>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="1"/>
@@ -7752,10 +7759,10 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="R65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
@@ -7785,7 +7792,7 @@
         <f>IF(Aufwandsplan!E65&lt;&gt;0, Aufwandsplan!E65, "")</f>
         <v>11</v>
       </c>
-      <c r="G66" s="22">
+      <c r="G66" s="44">
         <f>IF(Aufwandsplan!F65&lt;&gt;0, Aufwandsplan!F65, "")</f>
         <v>1</v>
       </c>
@@ -7801,7 +7808,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -7832,7 +7839,7 @@
         <f>IF(Aufwandsplan!E66&lt;&gt;0, Aufwandsplan!E66, "")</f>
         <v>5</v>
       </c>
-      <c r="G67" s="22" t="str">
+      <c r="G67" s="44" t="str">
         <f>IF(Aufwandsplan!F66&lt;&gt;0, Aufwandsplan!F66, "")</f>
         <v/>
       </c>
@@ -7848,7 +7855,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1" t="s">
-        <v>217</v>
+        <v>87</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -7877,11 +7884,11 @@
       </c>
       <c r="F68" s="22">
         <f>IF(Aufwandsplan!E67&lt;&gt;0, Aufwandsplan!E67, "")</f>
-        <v>12</v>
-      </c>
-      <c r="G68" s="22" t="str">
+        <v>10</v>
+      </c>
+      <c r="G68" s="44">
         <f>IF(Aufwandsplan!F67&lt;&gt;0, Aufwandsplan!F67, "")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="H68" s="7"/>
       <c r="I68" s="1"/>
@@ -7894,7 +7901,9 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
+      <c r="S68" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="T68" s="1" t="s">
         <v>116</v>
       </c>
@@ -7926,7 +7935,7 @@
         <f>IF(Aufwandsplan!E68&lt;&gt;0, Aufwandsplan!E68, "")</f>
         <v>12</v>
       </c>
-      <c r="G69" s="22" t="str">
+      <c r="G69" s="44" t="str">
         <f>IF(Aufwandsplan!F68&lt;&gt;0, Aufwandsplan!F68, "")</f>
         <v/>
       </c>
@@ -7973,7 +7982,7 @@
         <f>IF(Aufwandsplan!E69&lt;&gt;0, Aufwandsplan!E69, "")</f>
         <v>2</v>
       </c>
-      <c r="G70" s="22">
+      <c r="G70" s="44">
         <f>IF(Aufwandsplan!F69&lt;&gt;0, Aufwandsplan!F69, "")</f>
         <v>10</v>
       </c>
@@ -8020,7 +8029,7 @@
         <f>IF(Aufwandsplan!E70&lt;&gt;0, Aufwandsplan!E70, "")</f>
         <v>11</v>
       </c>
-      <c r="G71" s="22">
+      <c r="G71" s="44">
         <f>IF(Aufwandsplan!F70&lt;&gt;0, Aufwandsplan!F70, "")</f>
         <v>-11</v>
       </c>
@@ -8034,13 +8043,11 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
-      <c r="R71" s="1" t="s">
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="S71" t="s">
-        <v>116</v>
-      </c>
-      <c r="T71" s="1"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
@@ -8069,7 +8076,7 @@
         <f>IF(Aufwandsplan!E71&lt;&gt;0, Aufwandsplan!E71, "")</f>
         <v>12</v>
       </c>
-      <c r="G72" s="22" t="str">
+      <c r="G72" s="44" t="str">
         <f>IF(Aufwandsplan!F71&lt;&gt;0, Aufwandsplan!F71, "")</f>
         <v/>
       </c>
@@ -8083,8 +8090,12 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
+      <c r="R72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S72" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
@@ -8112,11 +8123,11 @@
       </c>
       <c r="F73" s="22">
         <f>IF(Aufwandsplan!E72&lt;&gt;0, Aufwandsplan!E72, "")</f>
-        <v>57</v>
-      </c>
-      <c r="G73" s="22">
+        <v>37</v>
+      </c>
+      <c r="G73" s="44">
         <f>IF(Aufwandsplan!F72&lt;&gt;0, Aufwandsplan!F72, "")</f>
-        <v>-35</v>
+        <v>-15</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="1"/>
@@ -8161,7 +8172,7 @@
         <f>IF(Aufwandsplan!E73&lt;&gt;0, Aufwandsplan!E73, "")</f>
         <v>7</v>
       </c>
-      <c r="G74" s="22">
+      <c r="G74" s="44">
         <f>IF(Aufwandsplan!F73&lt;&gt;0, Aufwandsplan!F73, "")</f>
         <v>-7</v>
       </c>
@@ -8206,11 +8217,11 @@
       </c>
       <c r="F75" s="22">
         <f>IF(Aufwandsplan!E74&lt;&gt;0, Aufwandsplan!E74, "")</f>
-        <v>13</v>
-      </c>
-      <c r="G75" s="22">
+        <v>8</v>
+      </c>
+      <c r="G75" s="44">
         <f>IF(Aufwandsplan!F74&lt;&gt;0, Aufwandsplan!F74, "")</f>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="1"/>
@@ -8255,7 +8266,7 @@
         <f>IF(Aufwandsplan!E75&lt;&gt;0, Aufwandsplan!E75, "")</f>
         <v>8</v>
       </c>
-      <c r="G76" s="22">
+      <c r="G76" s="44">
         <f>IF(Aufwandsplan!F75&lt;&gt;0, Aufwandsplan!F75, "")</f>
         <v>-8</v>
       </c>
@@ -8300,11 +8311,11 @@
       </c>
       <c r="F77" s="22">
         <f>IF(Aufwandsplan!E76&lt;&gt;0, Aufwandsplan!E76, "")</f>
-        <v>16</v>
-      </c>
-      <c r="G77" s="22">
+        <v>15</v>
+      </c>
+      <c r="G77" s="44">
         <f>IF(Aufwandsplan!F76&lt;&gt;0, Aufwandsplan!F76, "")</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="1"/>
@@ -8317,11 +8328,12 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
       <c r="T77" s="1"/>
-      <c r="U77" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="V77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
       <c r="Y77" s="1"/>
@@ -8346,13 +8358,13 @@
       </c>
       <c r="F78" s="22">
         <f>IF(Aufwandsplan!E77&lt;&gt;0, Aufwandsplan!E77, "")</f>
-        <v>15</v>
-      </c>
-      <c r="G78" s="22">
+        <v>10</v>
+      </c>
+      <c r="G78" s="44">
         <f>IF(Aufwandsplan!F77&lt;&gt;0, Aufwandsplan!F77, "")</f>
-        <v>-15</v>
-      </c>
-      <c r="H78" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="H78" s="7"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
@@ -8366,7 +8378,9 @@
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
-      <c r="V78" s="1"/>
+      <c r="V78" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
       <c r="Y78" s="1"/>
@@ -8391,13 +8405,13 @@
       </c>
       <c r="F79" s="22">
         <f>IF(Aufwandsplan!E78&lt;&gt;0, Aufwandsplan!E78, "")</f>
-        <v>12</v>
-      </c>
-      <c r="G79" s="22">
+        <v>11</v>
+      </c>
+      <c r="G79" s="44">
         <f>IF(Aufwandsplan!F78&lt;&gt;0, Aufwandsplan!F78, "")</f>
-        <v>-12</v>
-      </c>
-      <c r="H79" s="1"/>
+        <v>-11</v>
+      </c>
+      <c r="H79" s="7"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -8411,7 +8425,9 @@
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
-      <c r="V79" s="1"/>
+      <c r="V79" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
       <c r="Y79" s="1"/>
@@ -8436,13 +8452,13 @@
       </c>
       <c r="F80" s="22">
         <f>IF(Aufwandsplan!E79&lt;&gt;0, Aufwandsplan!E79, "")</f>
-        <v>15</v>
-      </c>
-      <c r="G80" s="22">
+        <v>11</v>
+      </c>
+      <c r="G80" s="44">
         <f>IF(Aufwandsplan!F79&lt;&gt;0, Aufwandsplan!F79, "")</f>
-        <v>-15</v>
-      </c>
-      <c r="H80" s="1"/>
+        <v>-11</v>
+      </c>
+      <c r="H80" s="7"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -8457,11 +8473,13 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
-      <c r="W80" s="1"/>
+      <c r="W80" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="X80" s="1"/>
       <c r="Y80" s="1"/>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="22" t="str">
         <f>IF(Aufwandsplan!A80&lt;&gt;0, Aufwandsplan!A80, "")</f>
         <v>F2.18</v>
@@ -8483,11 +8501,11 @@
         <f>IF(Aufwandsplan!E80&lt;&gt;0, Aufwandsplan!E80, "")</f>
         <v>10</v>
       </c>
-      <c r="G81" s="22">
+      <c r="G81" s="44">
         <f>IF(Aufwandsplan!F80&lt;&gt;0, Aufwandsplan!F80, "")</f>
         <v>2</v>
       </c>
-      <c r="H81" s="1"/>
+      <c r="H81" s="7"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -8502,11 +8520,13 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
-      <c r="W81" s="1"/>
+      <c r="W81" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="X81" s="1"/>
       <c r="Y81" s="1"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="22" t="str">
         <f>IF(Aufwandsplan!A81&lt;&gt;0, Aufwandsplan!A81, "")</f>
         <v>F2.19</v>
@@ -8528,11 +8548,11 @@
         <f>IF(Aufwandsplan!E81&lt;&gt;0, Aufwandsplan!E81, "")</f>
         <v>10</v>
       </c>
-      <c r="G82" s="22">
+      <c r="G82" s="44">
         <f>IF(Aufwandsplan!F81&lt;&gt;0, Aufwandsplan!F81, "")</f>
         <v>2</v>
       </c>
-      <c r="H82" s="1"/>
+      <c r="H82" s="7"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -8547,11 +8567,13 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
-      <c r="W82" s="1"/>
+      <c r="W82" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="X82" s="1"/>
       <c r="Y82" s="1"/>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="22" t="str">
         <f>IF(Aufwandsplan!A82&lt;&gt;0, Aufwandsplan!A82, "")</f>
         <v>F2.20</v>
@@ -8573,11 +8595,11 @@
         <f>IF(Aufwandsplan!E82&lt;&gt;0, Aufwandsplan!E82, "")</f>
         <v>13</v>
       </c>
-      <c r="G83" s="22">
+      <c r="G83" s="44">
         <f>IF(Aufwandsplan!F82&lt;&gt;0, Aufwandsplan!F82, "")</f>
         <v>-1</v>
       </c>
-      <c r="H83" s="1"/>
+      <c r="H83" s="7"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -8588,15 +8610,17 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
-      <c r="S83" s="25"/>
+      <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
-      <c r="X83" s="1"/>
+      <c r="X83" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="Y83" s="1"/>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="22" t="str">
         <f>IF(Aufwandsplan!A83&lt;&gt;0, Aufwandsplan!A83, "")</f>
         <v>F2.21</v>
@@ -8616,13 +8640,13 @@
       </c>
       <c r="F84" s="22">
         <f>IF(Aufwandsplan!E83&lt;&gt;0, Aufwandsplan!E83, "")</f>
-        <v>8</v>
-      </c>
-      <c r="G84" s="22">
+        <v>7</v>
+      </c>
+      <c r="G84" s="44">
         <f>IF(Aufwandsplan!F83&lt;&gt;0, Aufwandsplan!F83, "")</f>
-        <v>-8</v>
-      </c>
-      <c r="H84" s="1"/>
+        <v>-7</v>
+      </c>
+      <c r="H84" s="7"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
@@ -8634,16 +8658,16 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
-      <c r="T84" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="T84" s="1"/>
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
-      <c r="X84" s="1"/>
+      <c r="X84" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="Y84" s="1"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="str">
         <f>IF(Aufwandsplan!A84&lt;&gt;0, Aufwandsplan!A84, "")</f>
         <v>F3</v>
@@ -8665,11 +8689,11 @@
         <f>IF(Aufwandsplan!E84&lt;&gt;0, Aufwandsplan!E84, "")</f>
         <v/>
       </c>
-      <c r="G85" s="22" t="str">
+      <c r="G85" s="44" t="str">
         <f>IF(Aufwandsplan!F84&lt;&gt;0, Aufwandsplan!F84, "")</f>
         <v/>
       </c>
-      <c r="H85" s="1"/>
+      <c r="H85" s="7"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
@@ -8680,19 +8704,15 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
-      <c r="S85" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="T85" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="S85" s="25"/>
+      <c r="T85" s="1"/>
       <c r="U85" s="1"/>
-      <c r="V85" s="1"/>
+      <c r="V85" s="29"/>
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
       <c r="Y85" s="1"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="22" t="str">
         <f>IF(Aufwandsplan!A85&lt;&gt;0, Aufwandsplan!A85, "")</f>
         <v>F3.1</v>
@@ -8714,11 +8734,11 @@
         <f>IF(Aufwandsplan!E85&lt;&gt;0, Aufwandsplan!E85, "")</f>
         <v>20</v>
       </c>
-      <c r="G86" s="22">
+      <c r="G86" s="44">
         <f>IF(Aufwandsplan!F85&lt;&gt;0, Aufwandsplan!F85, "")</f>
         <v>5</v>
       </c>
-      <c r="H86" s="1"/>
+      <c r="H86" s="7"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -8729,7 +8749,9 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
+      <c r="S86" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
@@ -8737,7 +8759,7 @@
       <c r="X86" s="1"/>
       <c r="Y86" s="1"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="str">
         <f>IF(Aufwandsplan!A86&lt;&gt;0, Aufwandsplan!A86, "")</f>
         <v>F3.2</v>
@@ -8759,11 +8781,11 @@
         <f>IF(Aufwandsplan!E86&lt;&gt;0, Aufwandsplan!E86, "")</f>
         <v>24</v>
       </c>
-      <c r="G87" s="22">
+      <c r="G87" s="44">
         <f>IF(Aufwandsplan!F86&lt;&gt;0, Aufwandsplan!F86, "")</f>
         <v>1</v>
       </c>
-      <c r="H87" s="1"/>
+      <c r="H87" s="7"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -8775,14 +8797,18 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
-      <c r="T87" s="1"/>
-      <c r="U87" s="1"/>
+      <c r="T87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U87" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
       <c r="Y87" s="1"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="22" t="str">
         <f>IF(Aufwandsplan!A87&lt;&gt;0, Aufwandsplan!A87, "")</f>
         <v>F3.3</v>
@@ -8802,13 +8828,13 @@
       </c>
       <c r="F88" s="22">
         <f>IF(Aufwandsplan!E87&lt;&gt;0, Aufwandsplan!E87, "")</f>
-        <v>30</v>
-      </c>
-      <c r="G88" s="22">
+        <v>28</v>
+      </c>
+      <c r="G88" s="44">
         <f>IF(Aufwandsplan!F87&lt;&gt;0, Aufwandsplan!F87, "")</f>
-        <v>-5</v>
-      </c>
-      <c r="H88" s="1"/>
+        <v>-3</v>
+      </c>
+      <c r="H88" s="7"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
@@ -8821,13 +8847,17 @@
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
-      <c r="U88" s="1"/>
-      <c r="V88" s="1"/>
+      <c r="U88" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V88" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
       <c r="Y88" s="1"/>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="str">
         <f>IF(Aufwandsplan!A88&lt;&gt;0, Aufwandsplan!A88, "")</f>
         <v>G1</v>
@@ -8851,11 +8881,11 @@
         <f>IF(Aufwandsplan!E88&lt;&gt;0, Aufwandsplan!E88, "")</f>
         <v>6</v>
       </c>
-      <c r="G89" s="22">
+      <c r="G89" s="44">
         <f>IF(Aufwandsplan!F88&lt;&gt;0, Aufwandsplan!F88, "")</f>
         <v>-2</v>
       </c>
-      <c r="H89" s="1"/>
+      <c r="H89" s="7"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
@@ -8872,9 +8902,11 @@
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
       <c r="X89" s="1"/>
-      <c r="Y89" s="1"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y89" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="22" t="str">
         <f>IF(Aufwandsplan!A89&lt;&gt;0, Aufwandsplan!A89, "")</f>
         <v>G2</v>
@@ -8896,11 +8928,11 @@
         <f>IF(Aufwandsplan!E89&lt;&gt;0, Aufwandsplan!E89, "")</f>
         <v>23</v>
       </c>
-      <c r="G90" s="22">
+      <c r="G90" s="44">
         <f>IF(Aufwandsplan!F89&lt;&gt;0, Aufwandsplan!F89, "")</f>
         <v>-13</v>
       </c>
-      <c r="H90" s="1"/>
+      <c r="H90" s="7"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -8917,9 +8949,11 @@
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
       <c r="X90" s="1"/>
-      <c r="Y90" s="1"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y90" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="22" t="str">
         <f>IF(Aufwandsplan!A90&lt;&gt;0, Aufwandsplan!A90, "")</f>
         <v>G3</v>
@@ -8941,11 +8975,11 @@
         <f>IF(Aufwandsplan!E90&lt;&gt;0, Aufwandsplan!E90, "")</f>
         <v>5</v>
       </c>
-      <c r="G91" s="22" t="str">
+      <c r="G91" s="44" t="str">
         <f>IF(Aufwandsplan!F90&lt;&gt;0, Aufwandsplan!F90, "")</f>
         <v/>
       </c>
-      <c r="H91" s="1"/>
+      <c r="H91" s="7"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
@@ -8962,9 +8996,17 @@
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
       <c r="X91" s="1"/>
-      <c r="Y91" s="1"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y91" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z92" s="45"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B93" s="26" t="s">
+        <v>250</v>
+      </c>
       <c r="F93" s="24" t="s">
         <v>210</v>
       </c>
@@ -9029,22 +9071,26 @@
       </c>
       <c r="V93" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W93" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X93" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y93" s="7">
+      <c r="Y93" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z93" s="45"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B94" s="28" t="s">
+        <v>249</v>
+      </c>
       <c r="G94" s="9" t="s">
         <v>89</v>
       </c>
@@ -9094,7 +9140,7 @@
       </c>
       <c r="S94" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T94" s="7">
         <f t="shared" si="1"/>
@@ -9102,11 +9148,11 @@
       </c>
       <c r="U94" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V94" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W94" s="7">
         <f t="shared" si="1"/>
@@ -9116,12 +9162,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y94" s="7">
+      <c r="Y94" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Z94" s="45"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G95" s="9" t="s">
         <v>217</v>
       </c>
@@ -9183,22 +9230,23 @@
       </c>
       <c r="V95" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W95" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X95" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y95" s="7">
+      <c r="Y95" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z95" s="45"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G96" s="9" t="s">
         <v>116</v>
       </c>
@@ -9252,30 +9300,31 @@
       </c>
       <c r="T96" s="7">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U96" s="7">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V96" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W96" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X96" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y96" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y96" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Z96" s="45"/>
+    </row>
+    <row r="97" spans="7:26" x14ac:dyDescent="0.25">
       <c r="G97" s="9" t="s">
         <v>121</v>
       </c>
@@ -9325,11 +9374,11 @@
       </c>
       <c r="S97" s="7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T97" s="7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U97" s="7">
         <f t="shared" si="4"/>
@@ -9347,34 +9396,14 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y97" s="7">
+      <c r="Y97" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B100" s="26" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="101" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B101" s="28" t="s">
-        <v>249</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="Z97" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="A2:A3"/>
@@ -9388,6 +9417,17 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>